<commit_message>
fetch data from url and format
</commit_message>
<xml_diff>
--- a/files/sic_look_up_list.xlsx
+++ b/files/sic_look_up_list.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daxia/DevProjects/PythonProject/SicProject/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFAB45EC-D44B-0144-9561-A9BF5C5B4C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D90768-7B75-EB49-BBA1-ACE8EE1F13D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12600" xr2:uid="{0209D9B5-85AC-49AC-92D9-C4E0A44ED0E5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{0209D9B5-85AC-49AC-92D9-C4E0A44ED0E5}"/>
   </bookViews>
   <sheets>
     <sheet name="SIC lookup list" sheetId="1" r:id="rId1"/>
+    <sheet name="list" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SIC lookup list'!$B$3:$D$279</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>ion Code</t>
   </si>
@@ -66,6 +67,9 @@
   </si>
   <si>
     <t>one digit</t>
+  </si>
+  <si>
+    <t>SIK</t>
   </si>
 </sst>
 </file>
@@ -420,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BA5331-FF6A-462D-B035-249272D95E6D}">
   <dimension ref="B2:I281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="B2:I279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4636,7 +4640,4195 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F5DF98-AC01-6741-89F0-018FFD1CD017}">
+  <dimension ref="A1:D277"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="35.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>6020</v>
+      </c>
+      <c r="B2">
+        <v>376</v>
+      </c>
+      <c r="C2">
+        <v>4.45</v>
+      </c>
+      <c r="D2">
+        <f ca="1">SUM(C2:$D$3)</f>
+        <v>4.45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>6798</v>
+      </c>
+      <c r="B3">
+        <v>354</v>
+      </c>
+      <c r="C3">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="D3">
+        <f ca="1">SUM(C$3:$D3)</f>
+        <v>8.64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3674</v>
+      </c>
+      <c r="B4">
+        <v>318</v>
+      </c>
+      <c r="C4">
+        <v>3.77</v>
+      </c>
+      <c r="D4">
+        <f ca="1">SUM(C$3:$D4)</f>
+        <v>12.41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1311</v>
+      </c>
+      <c r="B5">
+        <v>315</v>
+      </c>
+      <c r="C5">
+        <v>3.73</v>
+      </c>
+      <c r="D5">
+        <f ca="1">SUM(C$3:$D5)</f>
+        <v>16.14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2834</v>
+      </c>
+      <c r="B6">
+        <v>182</v>
+      </c>
+      <c r="C6">
+        <v>2.16</v>
+      </c>
+      <c r="D6">
+        <f ca="1">SUM(C$3:$D6)</f>
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6331</v>
+      </c>
+      <c r="B7">
+        <v>161</v>
+      </c>
+      <c r="C7">
+        <v>1.91</v>
+      </c>
+      <c r="D7">
+        <f ca="1">SUM(C$3:$D7)</f>
+        <v>20.21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4911</v>
+      </c>
+      <c r="B8">
+        <v>160</v>
+      </c>
+      <c r="C8">
+        <v>1.9</v>
+      </c>
+      <c r="D8">
+        <f ca="1">SUM(C$3:$D8)</f>
+        <v>22.11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7372</v>
+      </c>
+      <c r="B9">
+        <v>160</v>
+      </c>
+      <c r="C9">
+        <v>1.9</v>
+      </c>
+      <c r="D9">
+        <f ca="1">SUM(C$3:$D9)</f>
+        <v>24.009999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>4931</v>
+      </c>
+      <c r="B10">
+        <v>158</v>
+      </c>
+      <c r="C10">
+        <v>1.87</v>
+      </c>
+      <c r="D10">
+        <f ca="1">SUM(C$3:$D10)</f>
+        <v>25.88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7370</v>
+      </c>
+      <c r="B11">
+        <v>154</v>
+      </c>
+      <c r="C11">
+        <v>1.82</v>
+      </c>
+      <c r="D11">
+        <f ca="1">SUM(C$3:$D11)</f>
+        <v>27.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>6282</v>
+      </c>
+      <c r="B12">
+        <v>124</v>
+      </c>
+      <c r="C12">
+        <v>1.47</v>
+      </c>
+      <c r="D12">
+        <f ca="1">SUM(C$3:$D12)</f>
+        <v>29.169999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2836</v>
+      </c>
+      <c r="B13">
+        <v>101</v>
+      </c>
+      <c r="C13">
+        <v>1.2</v>
+      </c>
+      <c r="D13">
+        <f ca="1">SUM(C$3:$D13)</f>
+        <v>30.369999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>7374</v>
+      </c>
+      <c r="B14">
+        <v>99</v>
+      </c>
+      <c r="C14">
+        <v>1.17</v>
+      </c>
+      <c r="D14">
+        <f ca="1">SUM(C$3:$D14)</f>
+        <v>31.54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>5812</v>
+      </c>
+      <c r="B15">
+        <v>98</v>
+      </c>
+      <c r="C15">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="D15">
+        <f ca="1">SUM(C$3:$D15)</f>
+        <v>32.699999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>6211</v>
+      </c>
+      <c r="B16">
+        <v>97</v>
+      </c>
+      <c r="C16">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D16">
+        <f ca="1">SUM(C$3:$D16)</f>
+        <v>33.849999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1531</v>
+      </c>
+      <c r="B17">
+        <v>90</v>
+      </c>
+      <c r="C17">
+        <v>1.07</v>
+      </c>
+      <c r="D17">
+        <f ca="1">SUM(C$3:$D17)</f>
+        <v>34.919999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3714</v>
+      </c>
+      <c r="B18">
+        <v>88</v>
+      </c>
+      <c r="C18">
+        <v>1.04</v>
+      </c>
+      <c r="D18">
+        <f ca="1">SUM(C$3:$D18)</f>
+        <v>35.959999999999994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1381</v>
+      </c>
+      <c r="B19">
+        <v>84</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <f ca="1">SUM(C$3:$D19)</f>
+        <v>36.959999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>4924</v>
+      </c>
+      <c r="B20">
+        <v>73</v>
+      </c>
+      <c r="C20">
+        <v>0.86</v>
+      </c>
+      <c r="D20">
+        <f ca="1">SUM(C$3:$D20)</f>
+        <v>37.819999999999993</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>6311</v>
+      </c>
+      <c r="B21">
+        <v>73</v>
+      </c>
+      <c r="C21">
+        <v>0.86</v>
+      </c>
+      <c r="D21">
+        <f ca="1">SUM(C$3:$D21)</f>
+        <v>38.679999999999993</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2911</v>
+      </c>
+      <c r="B22">
+        <v>69</v>
+      </c>
+      <c r="C22">
+        <v>0.82</v>
+      </c>
+      <c r="D22">
+        <f ca="1">SUM(C$3:$D22)</f>
+        <v>39.499999999999993</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>4923</v>
+      </c>
+      <c r="B23">
+        <v>69</v>
+      </c>
+      <c r="C23">
+        <v>0.82</v>
+      </c>
+      <c r="D23">
+        <f ca="1">SUM(C$3:$D23)</f>
+        <v>40.319999999999993</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>6351</v>
+      </c>
+      <c r="B24">
+        <v>68</v>
+      </c>
+      <c r="C24">
+        <v>0.81</v>
+      </c>
+      <c r="D24">
+        <f ca="1">SUM(C$3:$D24)</f>
+        <v>41.129999999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3826</v>
+      </c>
+      <c r="B25">
+        <v>65</v>
+      </c>
+      <c r="C25">
+        <v>0.77</v>
+      </c>
+      <c r="D25">
+        <f ca="1">SUM(C$3:$D25)</f>
+        <v>41.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>4512</v>
+      </c>
+      <c r="B26">
+        <v>62</v>
+      </c>
+      <c r="C26">
+        <v>0.73</v>
+      </c>
+      <c r="D26">
+        <f ca="1">SUM(C$3:$D26)</f>
+        <v>42.629999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1389</v>
+      </c>
+      <c r="B27">
+        <v>60</v>
+      </c>
+      <c r="C27">
+        <v>0.71</v>
+      </c>
+      <c r="D27">
+        <f ca="1">SUM(C$3:$D27)</f>
+        <v>43.339999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>4833</v>
+      </c>
+      <c r="B28">
+        <v>57</v>
+      </c>
+      <c r="C28">
+        <v>0.68</v>
+      </c>
+      <c r="D28">
+        <f ca="1">SUM(C$3:$D28)</f>
+        <v>44.019999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>3572</v>
+      </c>
+      <c r="B29">
+        <v>56</v>
+      </c>
+      <c r="C29">
+        <v>0.66</v>
+      </c>
+      <c r="D29">
+        <f ca="1">SUM(C$3:$D29)</f>
+        <v>44.679999999999993</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>3576</v>
+      </c>
+      <c r="B30">
+        <v>56</v>
+      </c>
+      <c r="C30">
+        <v>0.66</v>
+      </c>
+      <c r="D30">
+        <f ca="1">SUM(C$3:$D30)</f>
+        <v>45.339999999999989</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>4813</v>
+      </c>
+      <c r="B31">
+        <v>56</v>
+      </c>
+      <c r="C31">
+        <v>0.66</v>
+      </c>
+      <c r="D31">
+        <f ca="1">SUM(C$3:$D31)</f>
+        <v>45.999999999999986</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>6324</v>
+      </c>
+      <c r="B32">
+        <v>56</v>
+      </c>
+      <c r="C32">
+        <v>0.66</v>
+      </c>
+      <c r="D32">
+        <f ca="1">SUM(C$3:$D32)</f>
+        <v>46.659999999999982</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>4812</v>
+      </c>
+      <c r="B33">
+        <v>55</v>
+      </c>
+      <c r="C33">
+        <v>0.65</v>
+      </c>
+      <c r="D33">
+        <f ca="1">SUM(C$3:$D33)</f>
+        <v>47.309999999999981</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3312</v>
+      </c>
+      <c r="B34">
+        <v>54</v>
+      </c>
+      <c r="C34">
+        <v>0.64</v>
+      </c>
+      <c r="D34">
+        <f ca="1">SUM(C$3:$D34)</f>
+        <v>47.949999999999982</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>7990</v>
+      </c>
+      <c r="B35">
+        <v>50</v>
+      </c>
+      <c r="C35">
+        <v>0.59</v>
+      </c>
+      <c r="D35">
+        <f ca="1">SUM(C$3:$D35)</f>
+        <v>48.539999999999985</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3533</v>
+      </c>
+      <c r="B36">
+        <v>49</v>
+      </c>
+      <c r="C36">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D36">
+        <f ca="1">SUM(C$3:$D36)</f>
+        <v>49.119999999999983</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>6141</v>
+      </c>
+      <c r="B37">
+        <v>49</v>
+      </c>
+      <c r="C37">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D37">
+        <f ca="1">SUM(C$3:$D37)</f>
+        <v>49.699999999999982</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>3812</v>
+      </c>
+      <c r="B38">
+        <v>48</v>
+      </c>
+      <c r="C38">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D38">
+        <f ca="1">SUM(C$3:$D38)</f>
+        <v>50.269999999999982</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2860</v>
+      </c>
+      <c r="B39">
+        <v>47</v>
+      </c>
+      <c r="C39">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D39">
+        <f ca="1">SUM(C$3:$D39)</f>
+        <v>50.829999999999984</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3663</v>
+      </c>
+      <c r="B40">
+        <v>47</v>
+      </c>
+      <c r="C40">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D40">
+        <f ca="1">SUM(C$3:$D40)</f>
+        <v>51.389999999999986</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>3561</v>
+      </c>
+      <c r="B41">
+        <v>46</v>
+      </c>
+      <c r="C41">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D41">
+        <f ca="1">SUM(C$3:$D41)</f>
+        <v>51.939999999999984</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>5311</v>
+      </c>
+      <c r="B42">
+        <v>46</v>
+      </c>
+      <c r="C42">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D42">
+        <f ca="1">SUM(C$3:$D42)</f>
+        <v>52.489999999999981</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2890</v>
+      </c>
+      <c r="B43">
+        <v>45</v>
+      </c>
+      <c r="C43">
+        <v>0.53</v>
+      </c>
+      <c r="D43">
+        <f ca="1">SUM(C$3:$D43)</f>
+        <v>53.019999999999982</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>4011</v>
+      </c>
+      <c r="B44">
+        <v>45</v>
+      </c>
+      <c r="C44">
+        <v>0.53</v>
+      </c>
+      <c r="D44">
+        <f ca="1">SUM(C$3:$D44)</f>
+        <v>53.549999999999983</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>8200</v>
+      </c>
+      <c r="B45">
+        <v>45</v>
+      </c>
+      <c r="C45">
+        <v>0.53</v>
+      </c>
+      <c r="D45">
+        <f ca="1">SUM(C$3:$D45)</f>
+        <v>54.079999999999984</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2810</v>
+      </c>
+      <c r="B46">
+        <v>44</v>
+      </c>
+      <c r="C46">
+        <v>0.52</v>
+      </c>
+      <c r="D46">
+        <f ca="1">SUM(C$3:$D46)</f>
+        <v>54.599999999999987</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2870</v>
+      </c>
+      <c r="B47">
+        <v>42</v>
+      </c>
+      <c r="C47">
+        <v>0.5</v>
+      </c>
+      <c r="D47">
+        <f ca="1">SUM(C$3:$D47)</f>
+        <v>55.099999999999987</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>6411</v>
+      </c>
+      <c r="B48">
+        <v>42</v>
+      </c>
+      <c r="C48">
+        <v>0.5</v>
+      </c>
+      <c r="D48">
+        <f ca="1">SUM(C$3:$D48)</f>
+        <v>55.599999999999987</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>3577</v>
+      </c>
+      <c r="B49">
+        <v>41</v>
+      </c>
+      <c r="C49">
+        <v>0.49</v>
+      </c>
+      <c r="D49">
+        <f ca="1">SUM(C$3:$D49)</f>
+        <v>56.089999999999989</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>7373</v>
+      </c>
+      <c r="B50">
+        <v>41</v>
+      </c>
+      <c r="C50">
+        <v>0.49</v>
+      </c>
+      <c r="D50">
+        <f ca="1">SUM(C$3:$D50)</f>
+        <v>56.579999999999991</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1220</v>
+      </c>
+      <c r="B51">
+        <v>39</v>
+      </c>
+      <c r="C51">
+        <v>0.46</v>
+      </c>
+      <c r="D51">
+        <f ca="1">SUM(C$3:$D51)</f>
+        <v>57.039999999999992</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2300</v>
+      </c>
+      <c r="B52">
+        <v>39</v>
+      </c>
+      <c r="C52">
+        <v>0.46</v>
+      </c>
+      <c r="D52">
+        <f ca="1">SUM(C$3:$D52)</f>
+        <v>57.499999999999993</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>3540</v>
+      </c>
+      <c r="B53">
+        <v>39</v>
+      </c>
+      <c r="C53">
+        <v>0.46</v>
+      </c>
+      <c r="D53">
+        <f ca="1">SUM(C$3:$D53)</f>
+        <v>57.959999999999994</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>3661</v>
+      </c>
+      <c r="B54">
+        <v>39</v>
+      </c>
+      <c r="C54">
+        <v>0.46</v>
+      </c>
+      <c r="D54">
+        <f ca="1">SUM(C$3:$D54)</f>
+        <v>58.419999999999995</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>3845</v>
+      </c>
+      <c r="B55">
+        <v>39</v>
+      </c>
+      <c r="C55">
+        <v>0.46</v>
+      </c>
+      <c r="D55">
+        <f ca="1">SUM(C$3:$D55)</f>
+        <v>58.879999999999995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>7389</v>
+      </c>
+      <c r="B56">
+        <v>39</v>
+      </c>
+      <c r="C56">
+        <v>0.46</v>
+      </c>
+      <c r="D56">
+        <f ca="1">SUM(C$3:$D56)</f>
+        <v>59.339999999999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>9995</v>
+      </c>
+      <c r="B57">
+        <v>39</v>
+      </c>
+      <c r="C57">
+        <v>0.46</v>
+      </c>
+      <c r="D57">
+        <f ca="1">SUM(C$3:$D57)</f>
+        <v>59.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>5621</v>
+      </c>
+      <c r="B58">
+        <v>38</v>
+      </c>
+      <c r="C58">
+        <v>0.45</v>
+      </c>
+      <c r="D58">
+        <f ca="1">SUM(C$3:$D58)</f>
+        <v>60.25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>6321</v>
+      </c>
+      <c r="B59">
+        <v>38</v>
+      </c>
+      <c r="C59">
+        <v>0.45</v>
+      </c>
+      <c r="D59">
+        <f ca="1">SUM(C$3:$D59)</f>
+        <v>60.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>5122</v>
+      </c>
+      <c r="B60">
+        <v>37</v>
+      </c>
+      <c r="C60">
+        <v>0.44</v>
+      </c>
+      <c r="D60">
+        <f ca="1">SUM(C$3:$D60)</f>
+        <v>61.14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>7323</v>
+      </c>
+      <c r="B61">
+        <v>37</v>
+      </c>
+      <c r="C61">
+        <v>0.44</v>
+      </c>
+      <c r="D61">
+        <f ca="1">SUM(C$3:$D61)</f>
+        <v>61.58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>2000</v>
+      </c>
+      <c r="B62">
+        <v>36</v>
+      </c>
+      <c r="C62">
+        <v>0.43</v>
+      </c>
+      <c r="D62">
+        <f ca="1">SUM(C$3:$D62)</f>
+        <v>62.01</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>4400</v>
+      </c>
+      <c r="B63">
+        <v>36</v>
+      </c>
+      <c r="C63">
+        <v>0.43</v>
+      </c>
+      <c r="D63">
+        <f ca="1">SUM(C$3:$D63)</f>
+        <v>62.44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>2040</v>
+      </c>
+      <c r="B64">
+        <v>35</v>
+      </c>
+      <c r="C64">
+        <v>0.41</v>
+      </c>
+      <c r="D64">
+        <f ca="1">SUM(C$3:$D64)</f>
+        <v>62.849999999999994</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>3510</v>
+      </c>
+      <c r="B65">
+        <v>35</v>
+      </c>
+      <c r="C65">
+        <v>0.41</v>
+      </c>
+      <c r="D65">
+        <f ca="1">SUM(C$3:$D65)</f>
+        <v>63.259999999999991</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>3585</v>
+      </c>
+      <c r="B66">
+        <v>35</v>
+      </c>
+      <c r="C66">
+        <v>0.41</v>
+      </c>
+      <c r="D66">
+        <f ca="1">SUM(C$3:$D66)</f>
+        <v>63.669999999999987</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>5912</v>
+      </c>
+      <c r="B67">
+        <v>35</v>
+      </c>
+      <c r="C67">
+        <v>0.41</v>
+      </c>
+      <c r="D67">
+        <f ca="1">SUM(C$3:$D67)</f>
+        <v>64.079999999999984</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>8062</v>
+      </c>
+      <c r="B68">
+        <v>35</v>
+      </c>
+      <c r="C68">
+        <v>0.41</v>
+      </c>
+      <c r="D68">
+        <f ca="1">SUM(C$3:$D68)</f>
+        <v>64.489999999999981</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>2844</v>
+      </c>
+      <c r="B69">
+        <v>34</v>
+      </c>
+      <c r="C69">
+        <v>0.4</v>
+      </c>
+      <c r="D69">
+        <f ca="1">SUM(C$3:$D69)</f>
+        <v>64.889999999999986</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>3711</v>
+      </c>
+      <c r="B70">
+        <v>34</v>
+      </c>
+      <c r="C70">
+        <v>0.4</v>
+      </c>
+      <c r="D70">
+        <f ca="1">SUM(C$3:$D70)</f>
+        <v>65.289999999999992</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>6200</v>
+      </c>
+      <c r="B71">
+        <v>34</v>
+      </c>
+      <c r="C71">
+        <v>0.4</v>
+      </c>
+      <c r="D71">
+        <f ca="1">SUM(C$3:$D71)</f>
+        <v>65.69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>1600</v>
+      </c>
+      <c r="B72">
+        <v>33</v>
+      </c>
+      <c r="C72">
+        <v>0.39</v>
+      </c>
+      <c r="D72">
+        <f ca="1">SUM(C$3:$D72)</f>
+        <v>66.08</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>4888</v>
+      </c>
+      <c r="B73">
+        <v>32</v>
+      </c>
+      <c r="C73">
+        <v>0.38</v>
+      </c>
+      <c r="D73">
+        <f ca="1">SUM(C$3:$D73)</f>
+        <v>66.459999999999994</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>6799</v>
+      </c>
+      <c r="B74">
+        <v>32</v>
+      </c>
+      <c r="C74">
+        <v>0.38</v>
+      </c>
+      <c r="D74">
+        <f ca="1">SUM(C$3:$D74)</f>
+        <v>66.839999999999989</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>2835</v>
+      </c>
+      <c r="B75">
+        <v>31</v>
+      </c>
+      <c r="C75">
+        <v>0.37</v>
+      </c>
+      <c r="D75">
+        <f ca="1">SUM(C$3:$D75)</f>
+        <v>67.209999999999994</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>2820</v>
+      </c>
+      <c r="B76">
+        <v>30</v>
+      </c>
+      <c r="C76">
+        <v>0.36</v>
+      </c>
+      <c r="D76">
+        <f ca="1">SUM(C$3:$D76)</f>
+        <v>67.569999999999993</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>2851</v>
+      </c>
+      <c r="B77">
+        <v>30</v>
+      </c>
+      <c r="C77">
+        <v>0.36</v>
+      </c>
+      <c r="D77">
+        <f ca="1">SUM(C$3:$D77)</f>
+        <v>67.929999999999993</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>3721</v>
+      </c>
+      <c r="B78">
+        <v>30</v>
+      </c>
+      <c r="C78">
+        <v>0.36</v>
+      </c>
+      <c r="D78">
+        <f ca="1">SUM(C$3:$D78)</f>
+        <v>68.289999999999992</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>8742</v>
+      </c>
+      <c r="B79">
+        <v>30</v>
+      </c>
+      <c r="C79">
+        <v>0.36</v>
+      </c>
+      <c r="D79">
+        <f ca="1">SUM(C$3:$D79)</f>
+        <v>68.649999999999991</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>2400</v>
+      </c>
+      <c r="B80">
+        <v>29</v>
+      </c>
+      <c r="C80">
+        <v>0.34</v>
+      </c>
+      <c r="D80">
+        <f ca="1">SUM(C$3:$D80)</f>
+        <v>68.989999999999995</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>3559</v>
+      </c>
+      <c r="B81">
+        <v>29</v>
+      </c>
+      <c r="C81">
+        <v>0.34</v>
+      </c>
+      <c r="D81">
+        <f ca="1">SUM(C$3:$D81)</f>
+        <v>69.33</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>4922</v>
+      </c>
+      <c r="B82">
+        <v>29</v>
+      </c>
+      <c r="C82">
+        <v>0.34</v>
+      </c>
+      <c r="D82">
+        <f ca="1">SUM(C$3:$D82)</f>
+        <v>69.67</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>5651</v>
+      </c>
+      <c r="B83">
+        <v>29</v>
+      </c>
+      <c r="C83">
+        <v>0.34</v>
+      </c>
+      <c r="D83">
+        <f ca="1">SUM(C$3:$D83)</f>
+        <v>70.010000000000005</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>3290</v>
+      </c>
+      <c r="B84">
+        <v>28</v>
+      </c>
+      <c r="C84">
+        <v>0.33</v>
+      </c>
+      <c r="D84">
+        <f ca="1">SUM(C$3:$D84)</f>
+        <v>70.34</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>2111</v>
+      </c>
+      <c r="B85">
+        <v>27</v>
+      </c>
+      <c r="C85">
+        <v>0.32</v>
+      </c>
+      <c r="D85">
+        <f ca="1">SUM(C$3:$D85)</f>
+        <v>70.66</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>3089</v>
+      </c>
+      <c r="B86">
+        <v>27</v>
+      </c>
+      <c r="C86">
+        <v>0.32</v>
+      </c>
+      <c r="D86">
+        <f ca="1">SUM(C$3:$D86)</f>
+        <v>70.97999999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>3411</v>
+      </c>
+      <c r="B87">
+        <v>27</v>
+      </c>
+      <c r="C87">
+        <v>0.32</v>
+      </c>
+      <c r="D87">
+        <f ca="1">SUM(C$3:$D87)</f>
+        <v>71.299999999999983</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>3672</v>
+      </c>
+      <c r="B88">
+        <v>27</v>
+      </c>
+      <c r="C88">
+        <v>0.32</v>
+      </c>
+      <c r="D88">
+        <f ca="1">SUM(C$3:$D88)</f>
+        <v>71.619999999999976</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>3728</v>
+      </c>
+      <c r="B89">
+        <v>27</v>
+      </c>
+      <c r="C89">
+        <v>0.32</v>
+      </c>
+      <c r="D89">
+        <f ca="1">SUM(C$3:$D89)</f>
+        <v>71.939999999999969</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>5331</v>
+      </c>
+      <c r="B90">
+        <v>27</v>
+      </c>
+      <c r="C90">
+        <v>0.32</v>
+      </c>
+      <c r="D90">
+        <f ca="1">SUM(C$3:$D90)</f>
+        <v>72.259999999999962</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>6794</v>
+      </c>
+      <c r="B91">
+        <v>27</v>
+      </c>
+      <c r="C91">
+        <v>0.32</v>
+      </c>
+      <c r="D91">
+        <f ca="1">SUM(C$3:$D91)</f>
+        <v>72.579999999999956</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>1400</v>
+      </c>
+      <c r="B92">
+        <v>26</v>
+      </c>
+      <c r="C92">
+        <v>0.31</v>
+      </c>
+      <c r="D92">
+        <f ca="1">SUM(C$3:$D92)</f>
+        <v>72.889999999999958</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>4991</v>
+      </c>
+      <c r="B93">
+        <v>26</v>
+      </c>
+      <c r="C93">
+        <v>0.31</v>
+      </c>
+      <c r="D93">
+        <f ca="1">SUM(C$3:$D93)</f>
+        <v>73.19999999999996</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>7011</v>
+      </c>
+      <c r="B94">
+        <v>26</v>
+      </c>
+      <c r="C94">
+        <v>0.31</v>
+      </c>
+      <c r="D94">
+        <f ca="1">SUM(C$3:$D94)</f>
+        <v>73.509999999999962</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>2631</v>
+      </c>
+      <c r="B95">
+        <v>25</v>
+      </c>
+      <c r="C95">
+        <v>0.3</v>
+      </c>
+      <c r="D95">
+        <f ca="1">SUM(C$3:$D95)</f>
+        <v>73.80999999999996</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>3570</v>
+      </c>
+      <c r="B96">
+        <v>25</v>
+      </c>
+      <c r="C96">
+        <v>0.3</v>
+      </c>
+      <c r="D96">
+        <f ca="1">SUM(C$3:$D96)</f>
+        <v>74.109999999999957</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>4841</v>
+      </c>
+      <c r="B97">
+        <v>25</v>
+      </c>
+      <c r="C97">
+        <v>0.3</v>
+      </c>
+      <c r="D97">
+        <f ca="1">SUM(C$3:$D97)</f>
+        <v>74.409999999999954</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>3841</v>
+      </c>
+      <c r="B98">
+        <v>24</v>
+      </c>
+      <c r="C98">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D98">
+        <f ca="1">SUM(C$3:$D98)</f>
+        <v>74.689999999999955</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>1000</v>
+      </c>
+      <c r="B99">
+        <v>23</v>
+      </c>
+      <c r="C99">
+        <v>0.27</v>
+      </c>
+      <c r="D99">
+        <f ca="1">SUM(C$3:$D99)</f>
+        <v>74.959999999999951</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>2086</v>
+      </c>
+      <c r="B100">
+        <v>23</v>
+      </c>
+      <c r="C100">
+        <v>0.27</v>
+      </c>
+      <c r="D100">
+        <f ca="1">SUM(C$3:$D100)</f>
+        <v>75.229999999999947</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>4213</v>
+      </c>
+      <c r="B101">
+        <v>23</v>
+      </c>
+      <c r="C101">
+        <v>0.27</v>
+      </c>
+      <c r="D101">
+        <f ca="1">SUM(C$3:$D101)</f>
+        <v>75.499999999999943</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>5961</v>
+      </c>
+      <c r="B102">
+        <v>23</v>
+      </c>
+      <c r="C102">
+        <v>0.27</v>
+      </c>
+      <c r="D102">
+        <f ca="1">SUM(C$3:$D102)</f>
+        <v>75.769999999999939</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>8711</v>
+      </c>
+      <c r="B103">
+        <v>23</v>
+      </c>
+      <c r="C103">
+        <v>0.27</v>
+      </c>
+      <c r="D103">
+        <f ca="1">SUM(C$3:$D103)</f>
+        <v>76.039999999999935</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>2670</v>
+      </c>
+      <c r="B104">
+        <v>22</v>
+      </c>
+      <c r="C104">
+        <v>0.26</v>
+      </c>
+      <c r="D104">
+        <f ca="1">SUM(C$3:$D104)</f>
+        <v>76.29999999999994</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>5940</v>
+      </c>
+      <c r="B105">
+        <v>22</v>
+      </c>
+      <c r="C105">
+        <v>0.26</v>
+      </c>
+      <c r="D105">
+        <f ca="1">SUM(C$3:$D105)</f>
+        <v>76.559999999999945</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>6531</v>
+      </c>
+      <c r="B106">
+        <v>22</v>
+      </c>
+      <c r="C106">
+        <v>0.26</v>
+      </c>
+      <c r="D106">
+        <f ca="1">SUM(C$3:$D106)</f>
+        <v>76.819999999999951</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>2011</v>
+      </c>
+      <c r="B107">
+        <v>21</v>
+      </c>
+      <c r="C107">
+        <v>0.25</v>
+      </c>
+      <c r="D107">
+        <f ca="1">SUM(C$3:$D107)</f>
+        <v>77.069999999999951</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>3640</v>
+      </c>
+      <c r="B108">
+        <v>21</v>
+      </c>
+      <c r="C108">
+        <v>0.25</v>
+      </c>
+      <c r="D108">
+        <f ca="1">SUM(C$3:$D108)</f>
+        <v>77.319999999999951</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>3823</v>
+      </c>
+      <c r="B109">
+        <v>21</v>
+      </c>
+      <c r="C109">
+        <v>0.25</v>
+      </c>
+      <c r="D109">
+        <f ca="1">SUM(C$3:$D109)</f>
+        <v>77.569999999999951</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>5211</v>
+      </c>
+      <c r="B110">
+        <v>21</v>
+      </c>
+      <c r="C110">
+        <v>0.25</v>
+      </c>
+      <c r="D110">
+        <f ca="1">SUM(C$3:$D110)</f>
+        <v>77.819999999999951</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>6035</v>
+      </c>
+      <c r="B111">
+        <v>21</v>
+      </c>
+      <c r="C111">
+        <v>0.25</v>
+      </c>
+      <c r="D111">
+        <f ca="1">SUM(C$3:$D111)</f>
+        <v>78.069999999999951</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>2650</v>
+      </c>
+      <c r="B112">
+        <v>20</v>
+      </c>
+      <c r="C112">
+        <v>0.24</v>
+      </c>
+      <c r="D112">
+        <f ca="1">SUM(C$3:$D112)</f>
+        <v>78.309999999999945</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>2711</v>
+      </c>
+      <c r="B113">
+        <v>20</v>
+      </c>
+      <c r="C113">
+        <v>0.24</v>
+      </c>
+      <c r="D113">
+        <f ca="1">SUM(C$3:$D113)</f>
+        <v>78.54999999999994</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>3420</v>
+      </c>
+      <c r="B114">
+        <v>20</v>
+      </c>
+      <c r="C114">
+        <v>0.24</v>
+      </c>
+      <c r="D114">
+        <f ca="1">SUM(C$3:$D114)</f>
+        <v>78.789999999999935</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>4953</v>
+      </c>
+      <c r="B115">
+        <v>20</v>
+      </c>
+      <c r="C115">
+        <v>0.24</v>
+      </c>
+      <c r="D115">
+        <f ca="1">SUM(C$3:$D115)</f>
+        <v>79.02999999999993</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>2030</v>
+      </c>
+      <c r="B116">
+        <v>19</v>
+      </c>
+      <c r="C116">
+        <v>0.23</v>
+      </c>
+      <c r="D116">
+        <f ca="1">SUM(C$3:$D116)</f>
+        <v>79.259999999999934</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>2060</v>
+      </c>
+      <c r="B117">
+        <v>19</v>
+      </c>
+      <c r="C117">
+        <v>0.23</v>
+      </c>
+      <c r="D117">
+        <f ca="1">SUM(C$3:$D117)</f>
+        <v>79.489999999999938</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>2531</v>
+      </c>
+      <c r="B118">
+        <v>19</v>
+      </c>
+      <c r="C118">
+        <v>0.23</v>
+      </c>
+      <c r="D118">
+        <f ca="1">SUM(C$3:$D118)</f>
+        <v>79.719999999999942</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>3350</v>
+      </c>
+      <c r="B119">
+        <v>19</v>
+      </c>
+      <c r="C119">
+        <v>0.23</v>
+      </c>
+      <c r="D119">
+        <f ca="1">SUM(C$3:$D119)</f>
+        <v>79.949999999999946</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>3490</v>
+      </c>
+      <c r="B120">
+        <v>19</v>
+      </c>
+      <c r="C120">
+        <v>0.23</v>
+      </c>
+      <c r="D120">
+        <f ca="1">SUM(C$3:$D120)</f>
+        <v>80.17999999999995</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>3523</v>
+      </c>
+      <c r="B121">
+        <v>19</v>
+      </c>
+      <c r="C121">
+        <v>0.23</v>
+      </c>
+      <c r="D121">
+        <f ca="1">SUM(C$3:$D121)</f>
+        <v>80.409999999999954</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>3578</v>
+      </c>
+      <c r="B122">
+        <v>19</v>
+      </c>
+      <c r="C122">
+        <v>0.23</v>
+      </c>
+      <c r="D122">
+        <f ca="1">SUM(C$3:$D122)</f>
+        <v>80.639999999999958</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>3743</v>
+      </c>
+      <c r="B123">
+        <v>19</v>
+      </c>
+      <c r="C123">
+        <v>0.23</v>
+      </c>
+      <c r="D123">
+        <f ca="1">SUM(C$3:$D123)</f>
+        <v>80.869999999999962</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>4832</v>
+      </c>
+      <c r="B124">
+        <v>19</v>
+      </c>
+      <c r="C124">
+        <v>0.23</v>
+      </c>
+      <c r="D124">
+        <f ca="1">SUM(C$3:$D124)</f>
+        <v>81.099999999999966</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>5045</v>
+      </c>
+      <c r="B125">
+        <v>19</v>
+      </c>
+      <c r="C125">
+        <v>0.23</v>
+      </c>
+      <c r="D125">
+        <f ca="1">SUM(C$3:$D125)</f>
+        <v>81.32999999999997</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>5065</v>
+      </c>
+      <c r="B126">
+        <v>19</v>
+      </c>
+      <c r="C126">
+        <v>0.23</v>
+      </c>
+      <c r="D126">
+        <f ca="1">SUM(C$3:$D126)</f>
+        <v>81.559999999999974</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>5411</v>
+      </c>
+      <c r="B127">
+        <v>19</v>
+      </c>
+      <c r="C127">
+        <v>0.23</v>
+      </c>
+      <c r="D127">
+        <f ca="1">SUM(C$3:$D127)</f>
+        <v>81.789999999999978</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>6099</v>
+      </c>
+      <c r="B128">
+        <v>19</v>
+      </c>
+      <c r="C128">
+        <v>0.23</v>
+      </c>
+      <c r="D128">
+        <f ca="1">SUM(C$3:$D128)</f>
+        <v>82.019999999999982</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>6111</v>
+      </c>
+      <c r="B129">
+        <v>19</v>
+      </c>
+      <c r="C129">
+        <v>0.23</v>
+      </c>
+      <c r="D129">
+        <f ca="1">SUM(C$3:$D129)</f>
+        <v>82.249999999999986</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>1040</v>
+      </c>
+      <c r="B130">
+        <v>18</v>
+      </c>
+      <c r="C130">
+        <v>0.21</v>
+      </c>
+      <c r="D130">
+        <f ca="1">SUM(C$3:$D130)</f>
+        <v>82.45999999999998</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>2621</v>
+      </c>
+      <c r="B131">
+        <v>18</v>
+      </c>
+      <c r="C131">
+        <v>0.21</v>
+      </c>
+      <c r="D131">
+        <f ca="1">SUM(C$3:$D131)</f>
+        <v>82.669999999999973</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>2833</v>
+      </c>
+      <c r="B132">
+        <v>18</v>
+      </c>
+      <c r="C132">
+        <v>0.21</v>
+      </c>
+      <c r="D132">
+        <f ca="1">SUM(C$3:$D132)</f>
+        <v>82.879999999999967</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>3011</v>
+      </c>
+      <c r="B133">
+        <v>18</v>
+      </c>
+      <c r="C133">
+        <v>0.21</v>
+      </c>
+      <c r="D133">
+        <f ca="1">SUM(C$3:$D133)</f>
+        <v>83.089999999999961</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>3100</v>
+      </c>
+      <c r="B134">
+        <v>18</v>
+      </c>
+      <c r="C134">
+        <v>0.21</v>
+      </c>
+      <c r="D134">
+        <f ca="1">SUM(C$3:$D134)</f>
+        <v>83.299999999999955</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>3569</v>
+      </c>
+      <c r="B135">
+        <v>18</v>
+      </c>
+      <c r="C135">
+        <v>0.21</v>
+      </c>
+      <c r="D135">
+        <f ca="1">SUM(C$3:$D135)</f>
+        <v>83.509999999999948</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>3990</v>
+      </c>
+      <c r="B136">
+        <v>18</v>
+      </c>
+      <c r="C136">
+        <v>0.21</v>
+      </c>
+      <c r="D136">
+        <f ca="1">SUM(C$3:$D136)</f>
+        <v>83.719999999999942</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>5000</v>
+      </c>
+      <c r="B137">
+        <v>18</v>
+      </c>
+      <c r="C137">
+        <v>0.21</v>
+      </c>
+      <c r="D137">
+        <f ca="1">SUM(C$3:$D137)</f>
+        <v>83.929999999999936</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>7510</v>
+      </c>
+      <c r="B138">
+        <v>18</v>
+      </c>
+      <c r="C138">
+        <v>0.21</v>
+      </c>
+      <c r="D138">
+        <f ca="1">SUM(C$3:$D138)</f>
+        <v>84.13999999999993</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>8731</v>
+      </c>
+      <c r="B139">
+        <v>18</v>
+      </c>
+      <c r="C139">
+        <v>0.21</v>
+      </c>
+      <c r="D139">
+        <f ca="1">SUM(C$3:$D139)</f>
+        <v>84.349999999999923</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>100</v>
+      </c>
+      <c r="B140">
+        <v>17</v>
+      </c>
+      <c r="C140">
+        <v>0.2</v>
+      </c>
+      <c r="D140">
+        <f ca="1">SUM(C$3:$D140)</f>
+        <v>84.549999999999926</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>2020</v>
+      </c>
+      <c r="B141">
+        <v>17</v>
+      </c>
+      <c r="C141">
+        <v>0.2</v>
+      </c>
+      <c r="D141">
+        <f ca="1">SUM(C$3:$D141)</f>
+        <v>84.749999999999929</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>2082</v>
+      </c>
+      <c r="B142">
+        <v>17</v>
+      </c>
+      <c r="C142">
+        <v>0.2</v>
+      </c>
+      <c r="D142">
+        <f ca="1">SUM(C$3:$D142)</f>
+        <v>84.949999999999932</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>2330</v>
+      </c>
+      <c r="B143">
+        <v>17</v>
+      </c>
+      <c r="C143">
+        <v>0.2</v>
+      </c>
+      <c r="D143">
+        <f ca="1">SUM(C$3:$D143)</f>
+        <v>85.149999999999935</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>2842</v>
+      </c>
+      <c r="B144">
+        <v>17</v>
+      </c>
+      <c r="C144">
+        <v>0.2</v>
+      </c>
+      <c r="D144">
+        <f ca="1">SUM(C$3:$D144)</f>
+        <v>85.349999999999937</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>3021</v>
+      </c>
+      <c r="B145">
+        <v>17</v>
+      </c>
+      <c r="C145">
+        <v>0.2</v>
+      </c>
+      <c r="D145">
+        <f ca="1">SUM(C$3:$D145)</f>
+        <v>85.54999999999994</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>3620</v>
+      </c>
+      <c r="B146">
+        <v>17</v>
+      </c>
+      <c r="C146">
+        <v>0.2</v>
+      </c>
+      <c r="D146">
+        <f ca="1">SUM(C$3:$D146)</f>
+        <v>85.749999999999943</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>3843</v>
+      </c>
+      <c r="B147">
+        <v>17</v>
+      </c>
+      <c r="C147">
+        <v>0.2</v>
+      </c>
+      <c r="D147">
+        <f ca="1">SUM(C$3:$D147)</f>
+        <v>85.949999999999946</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>4210</v>
+      </c>
+      <c r="B148">
+        <v>17</v>
+      </c>
+      <c r="C148">
+        <v>0.2</v>
+      </c>
+      <c r="D148">
+        <f ca="1">SUM(C$3:$D148)</f>
+        <v>86.149999999999949</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>5110</v>
+      </c>
+      <c r="B149">
+        <v>17</v>
+      </c>
+      <c r="C149">
+        <v>0.2</v>
+      </c>
+      <c r="D149">
+        <f ca="1">SUM(C$3:$D149)</f>
+        <v>86.349999999999952</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>5731</v>
+      </c>
+      <c r="B150">
+        <v>17</v>
+      </c>
+      <c r="C150">
+        <v>0.2</v>
+      </c>
+      <c r="D150">
+        <f ca="1">SUM(C$3:$D150)</f>
+        <v>86.549999999999955</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>7311</v>
+      </c>
+      <c r="B151">
+        <v>17</v>
+      </c>
+      <c r="C151">
+        <v>0.2</v>
+      </c>
+      <c r="D151">
+        <f ca="1">SUM(C$3:$D151)</f>
+        <v>86.749999999999957</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>7350</v>
+      </c>
+      <c r="B152">
+        <v>17</v>
+      </c>
+      <c r="C152">
+        <v>0.2</v>
+      </c>
+      <c r="D152">
+        <f ca="1">SUM(C$3:$D152)</f>
+        <v>86.94999999999996</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>2085</v>
+      </c>
+      <c r="B153">
+        <v>16</v>
+      </c>
+      <c r="C153">
+        <v>0.19</v>
+      </c>
+      <c r="D153">
+        <f ca="1">SUM(C$3:$D153)</f>
+        <v>87.139999999999958</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>2320</v>
+      </c>
+      <c r="B154">
+        <v>16</v>
+      </c>
+      <c r="C154">
+        <v>0.19</v>
+      </c>
+      <c r="D154">
+        <f ca="1">SUM(C$3:$D154)</f>
+        <v>87.329999999999956</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>3678</v>
+      </c>
+      <c r="B155">
+        <v>16</v>
+      </c>
+      <c r="C155">
+        <v>0.19</v>
+      </c>
+      <c r="D155">
+        <f ca="1">SUM(C$3:$D155)</f>
+        <v>87.519999999999953</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>5084</v>
+      </c>
+      <c r="B156">
+        <v>16</v>
+      </c>
+      <c r="C156">
+        <v>0.19</v>
+      </c>
+      <c r="D156">
+        <f ca="1">SUM(C$3:$D156)</f>
+        <v>87.709999999999951</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>5500</v>
+      </c>
+      <c r="B157">
+        <v>16</v>
+      </c>
+      <c r="C157">
+        <v>0.19</v>
+      </c>
+      <c r="D157">
+        <f ca="1">SUM(C$3:$D157)</f>
+        <v>87.899999999999949</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>5531</v>
+      </c>
+      <c r="B158">
+        <v>16</v>
+      </c>
+      <c r="C158">
+        <v>0.19</v>
+      </c>
+      <c r="D158">
+        <f ca="1">SUM(C$3:$D158)</f>
+        <v>88.089999999999947</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>5661</v>
+      </c>
+      <c r="B159">
+        <v>16</v>
+      </c>
+      <c r="C159">
+        <v>0.19</v>
+      </c>
+      <c r="D159">
+        <f ca="1">SUM(C$3:$D159)</f>
+        <v>88.279999999999944</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>6172</v>
+      </c>
+      <c r="B160">
+        <v>16</v>
+      </c>
+      <c r="C160">
+        <v>0.19</v>
+      </c>
+      <c r="D160">
+        <f ca="1">SUM(C$3:$D160)</f>
+        <v>88.469999999999942</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>7812</v>
+      </c>
+      <c r="B161">
+        <v>16</v>
+      </c>
+      <c r="C161">
+        <v>0.19</v>
+      </c>
+      <c r="D161">
+        <f ca="1">SUM(C$3:$D161)</f>
+        <v>88.65999999999994</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>2522</v>
+      </c>
+      <c r="B162">
+        <v>15</v>
+      </c>
+      <c r="C162">
+        <v>0.18</v>
+      </c>
+      <c r="D162">
+        <f ca="1">SUM(C$3:$D162)</f>
+        <v>88.839999999999947</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>3670</v>
+      </c>
+      <c r="B163">
+        <v>15</v>
+      </c>
+      <c r="C163">
+        <v>0.18</v>
+      </c>
+      <c r="D163">
+        <f ca="1">SUM(C$3:$D163)</f>
+        <v>89.019999999999953</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>5944</v>
+      </c>
+      <c r="B164">
+        <v>15</v>
+      </c>
+      <c r="C164">
+        <v>0.18</v>
+      </c>
+      <c r="D164">
+        <f ca="1">SUM(C$3:$D164)</f>
+        <v>89.19999999999996</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>8090</v>
+      </c>
+      <c r="B165">
+        <v>15</v>
+      </c>
+      <c r="C165">
+        <v>0.18</v>
+      </c>
+      <c r="D165">
+        <f ca="1">SUM(C$3:$D165)</f>
+        <v>89.379999999999967</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>2510</v>
+      </c>
+      <c r="B166">
+        <v>14</v>
+      </c>
+      <c r="C166">
+        <v>0.17</v>
+      </c>
+      <c r="D166">
+        <f ca="1">SUM(C$3:$D166)</f>
+        <v>89.549999999999969</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>3730</v>
+      </c>
+      <c r="B167">
+        <v>14</v>
+      </c>
+      <c r="C167">
+        <v>0.17</v>
+      </c>
+      <c r="D167">
+        <f ca="1">SUM(C$3:$D167)</f>
+        <v>89.71999999999997</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>4731</v>
+      </c>
+      <c r="B168">
+        <v>14</v>
+      </c>
+      <c r="C168">
+        <v>0.17</v>
+      </c>
+      <c r="D168">
+        <f ca="1">SUM(C$3:$D168)</f>
+        <v>89.889999999999972</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>8700</v>
+      </c>
+      <c r="B169">
+        <v>14</v>
+      </c>
+      <c r="C169">
+        <v>0.17</v>
+      </c>
+      <c r="D169">
+        <f ca="1">SUM(C$3:$D169)</f>
+        <v>90.059999999999974</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>3690</v>
+      </c>
+      <c r="B170">
+        <v>13</v>
+      </c>
+      <c r="C170">
+        <v>0.15</v>
+      </c>
+      <c r="D170">
+        <f ca="1">SUM(C$3:$D170)</f>
+        <v>90.20999999999998</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>4932</v>
+      </c>
+      <c r="B171">
+        <v>13</v>
+      </c>
+      <c r="C171">
+        <v>0.15</v>
+      </c>
+      <c r="D171">
+        <f ca="1">SUM(C$3:$D171)</f>
+        <v>90.359999999999985</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>5400</v>
+      </c>
+      <c r="B172">
+        <v>13</v>
+      </c>
+      <c r="C172">
+        <v>0.15</v>
+      </c>
+      <c r="D172">
+        <f ca="1">SUM(C$3:$D172)</f>
+        <v>90.509999999999991</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>7200</v>
+      </c>
+      <c r="B173">
+        <v>13</v>
+      </c>
+      <c r="C173">
+        <v>0.15</v>
+      </c>
+      <c r="D173">
+        <f ca="1">SUM(C$3:$D173)</f>
+        <v>90.66</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>8721</v>
+      </c>
+      <c r="B174">
+        <v>13</v>
+      </c>
+      <c r="C174">
+        <v>0.15</v>
+      </c>
+      <c r="D174">
+        <f ca="1">SUM(C$3:$D174)</f>
+        <v>90.81</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>3270</v>
+      </c>
+      <c r="B175">
+        <v>12</v>
+      </c>
+      <c r="C175">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D175">
+        <f ca="1">SUM(C$3:$D175)</f>
+        <v>90.95</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>3630</v>
+      </c>
+      <c r="B176">
+        <v>12</v>
+      </c>
+      <c r="C176">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D176">
+        <f ca="1">SUM(C$3:$D176)</f>
+        <v>91.09</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>3679</v>
+      </c>
+      <c r="B177">
+        <v>12</v>
+      </c>
+      <c r="C177">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D177">
+        <f ca="1">SUM(C$3:$D177)</f>
+        <v>91.23</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>4610</v>
+      </c>
+      <c r="B178">
+        <v>12</v>
+      </c>
+      <c r="C178">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D178">
+        <f ca="1">SUM(C$3:$D178)</f>
+        <v>91.37</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>9997</v>
+      </c>
+      <c r="B179">
+        <v>12</v>
+      </c>
+      <c r="C179">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D179">
+        <f ca="1">SUM(C$3:$D179)</f>
+        <v>91.51</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>2013</v>
+      </c>
+      <c r="B180">
+        <v>11</v>
+      </c>
+      <c r="C180">
+        <v>0.13</v>
+      </c>
+      <c r="D180">
+        <f ca="1">SUM(C$3:$D180)</f>
+        <v>91.64</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>6159</v>
+      </c>
+      <c r="B181">
+        <v>11</v>
+      </c>
+      <c r="C181">
+        <v>0.13</v>
+      </c>
+      <c r="D181">
+        <f ca="1">SUM(C$3:$D181)</f>
+        <v>91.77</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>1731</v>
+      </c>
+      <c r="B182">
+        <v>10</v>
+      </c>
+      <c r="C182">
+        <v>0.12</v>
+      </c>
+      <c r="D182">
+        <f ca="1">SUM(C$3:$D182)</f>
+        <v>91.89</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>2080</v>
+      </c>
+      <c r="B183">
+        <v>10</v>
+      </c>
+      <c r="C183">
+        <v>0.12</v>
+      </c>
+      <c r="D183">
+        <f ca="1">SUM(C$3:$D183)</f>
+        <v>92.01</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>2273</v>
+      </c>
+      <c r="B184">
+        <v>10</v>
+      </c>
+      <c r="C184">
+        <v>0.12</v>
+      </c>
+      <c r="D184">
+        <f ca="1">SUM(C$3:$D184)</f>
+        <v>92.13000000000001</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>2821</v>
+      </c>
+      <c r="B185">
+        <v>10</v>
+      </c>
+      <c r="C185">
+        <v>0.12</v>
+      </c>
+      <c r="D185">
+        <f ca="1">SUM(C$3:$D185)</f>
+        <v>92.250000000000014</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>3081</v>
+      </c>
+      <c r="B186">
+        <v>10</v>
+      </c>
+      <c r="C186">
+        <v>0.12</v>
+      </c>
+      <c r="D186">
+        <f ca="1">SUM(C$3:$D186)</f>
+        <v>92.370000000000019</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>3221</v>
+      </c>
+      <c r="B187">
+        <v>10</v>
+      </c>
+      <c r="C187">
+        <v>0.12</v>
+      </c>
+      <c r="D187">
+        <f ca="1">SUM(C$3:$D187)</f>
+        <v>92.490000000000023</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>3480</v>
+      </c>
+      <c r="B188">
+        <v>10</v>
+      </c>
+      <c r="C188">
+        <v>0.12</v>
+      </c>
+      <c r="D188">
+        <f ca="1">SUM(C$3:$D188)</f>
+        <v>92.610000000000028</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>3530</v>
+      </c>
+      <c r="B189">
+        <v>10</v>
+      </c>
+      <c r="C189">
+        <v>0.12</v>
+      </c>
+      <c r="D189">
+        <f ca="1">SUM(C$3:$D189)</f>
+        <v>92.730000000000032</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>3531</v>
+      </c>
+      <c r="B190">
+        <v>10</v>
+      </c>
+      <c r="C190">
+        <v>0.12</v>
+      </c>
+      <c r="D190">
+        <f ca="1">SUM(C$3:$D190)</f>
+        <v>92.850000000000037</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>3560</v>
+      </c>
+      <c r="B191">
+        <v>10</v>
+      </c>
+      <c r="C191">
+        <v>0.12</v>
+      </c>
+      <c r="D191">
+        <f ca="1">SUM(C$3:$D191)</f>
+        <v>92.970000000000041</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>3579</v>
+      </c>
+      <c r="B192">
+        <v>10</v>
+      </c>
+      <c r="C192">
+        <v>0.12</v>
+      </c>
+      <c r="D192">
+        <f ca="1">SUM(C$3:$D192)</f>
+        <v>93.090000000000046</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>3724</v>
+      </c>
+      <c r="B193">
+        <v>10</v>
+      </c>
+      <c r="C193">
+        <v>0.12</v>
+      </c>
+      <c r="D193">
+        <f ca="1">SUM(C$3:$D193)</f>
+        <v>93.210000000000051</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>3751</v>
+      </c>
+      <c r="B194">
+        <v>10</v>
+      </c>
+      <c r="C194">
+        <v>0.12</v>
+      </c>
+      <c r="D194">
+        <f ca="1">SUM(C$3:$D194)</f>
+        <v>93.330000000000055</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>3760</v>
+      </c>
+      <c r="B195">
+        <v>10</v>
+      </c>
+      <c r="C195">
+        <v>0.12</v>
+      </c>
+      <c r="D195">
+        <f ca="1">SUM(C$3:$D195)</f>
+        <v>93.45000000000006</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>3790</v>
+      </c>
+      <c r="B196">
+        <v>10</v>
+      </c>
+      <c r="C196">
+        <v>0.12</v>
+      </c>
+      <c r="D196">
+        <f ca="1">SUM(C$3:$D196)</f>
+        <v>93.570000000000064</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>3825</v>
+      </c>
+      <c r="B197">
+        <v>10</v>
+      </c>
+      <c r="C197">
+        <v>0.12</v>
+      </c>
+      <c r="D197">
+        <f ca="1">SUM(C$3:$D197)</f>
+        <v>93.690000000000069</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>3842</v>
+      </c>
+      <c r="B198">
+        <v>10</v>
+      </c>
+      <c r="C198">
+        <v>0.12</v>
+      </c>
+      <c r="D198">
+        <f ca="1">SUM(C$3:$D198)</f>
+        <v>93.810000000000073</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>3873</v>
+      </c>
+      <c r="B199">
+        <v>10</v>
+      </c>
+      <c r="C199">
+        <v>0.12</v>
+      </c>
+      <c r="D199">
+        <f ca="1">SUM(C$3:$D199)</f>
+        <v>93.930000000000078</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>3949</v>
+      </c>
+      <c r="B200">
+        <v>10</v>
+      </c>
+      <c r="C200">
+        <v>0.12</v>
+      </c>
+      <c r="D200">
+        <f ca="1">SUM(C$3:$D200)</f>
+        <v>94.050000000000082</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>5399</v>
+      </c>
+      <c r="B201">
+        <v>10</v>
+      </c>
+      <c r="C201">
+        <v>0.12</v>
+      </c>
+      <c r="D201">
+        <f ca="1">SUM(C$3:$D201)</f>
+        <v>94.170000000000087</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>6500</v>
+      </c>
+      <c r="B202">
+        <v>10</v>
+      </c>
+      <c r="C202">
+        <v>0.12</v>
+      </c>
+      <c r="D202">
+        <f ca="1">SUM(C$3:$D202)</f>
+        <v>94.290000000000092</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>2070</v>
+      </c>
+      <c r="B203">
+        <v>9</v>
+      </c>
+      <c r="C203">
+        <v>0.11</v>
+      </c>
+      <c r="D203">
+        <f ca="1">SUM(C$3:$D203)</f>
+        <v>94.400000000000091</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>2590</v>
+      </c>
+      <c r="B204">
+        <v>9</v>
+      </c>
+      <c r="C204">
+        <v>0.11</v>
+      </c>
+      <c r="D204">
+        <f ca="1">SUM(C$3:$D204)</f>
+        <v>94.51000000000009</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>2731</v>
+      </c>
+      <c r="B205">
+        <v>9</v>
+      </c>
+      <c r="C205">
+        <v>0.11</v>
+      </c>
+      <c r="D205">
+        <f ca="1">SUM(C$3:$D205)</f>
+        <v>94.62000000000009</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>2840</v>
+      </c>
+      <c r="B206">
+        <v>9</v>
+      </c>
+      <c r="C206">
+        <v>0.11</v>
+      </c>
+      <c r="D206">
+        <f ca="1">SUM(C$3:$D206)</f>
+        <v>94.730000000000089</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>3532</v>
+      </c>
+      <c r="B207">
+        <v>9</v>
+      </c>
+      <c r="C207">
+        <v>0.11</v>
+      </c>
+      <c r="D207">
+        <f ca="1">SUM(C$3:$D207)</f>
+        <v>94.840000000000089</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>3824</v>
+      </c>
+      <c r="B208">
+        <v>9</v>
+      </c>
+      <c r="C208">
+        <v>0.11</v>
+      </c>
+      <c r="D208">
+        <f ca="1">SUM(C$3:$D208)</f>
+        <v>94.950000000000088</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>3827</v>
+      </c>
+      <c r="B209">
+        <v>9</v>
+      </c>
+      <c r="C209">
+        <v>0.11</v>
+      </c>
+      <c r="D209">
+        <f ca="1">SUM(C$3:$D209)</f>
+        <v>95.060000000000088</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>3844</v>
+      </c>
+      <c r="B210">
+        <v>9</v>
+      </c>
+      <c r="C210">
+        <v>0.11</v>
+      </c>
+      <c r="D210">
+        <f ca="1">SUM(C$3:$D210)</f>
+        <v>95.170000000000087</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>3942</v>
+      </c>
+      <c r="B211">
+        <v>9</v>
+      </c>
+      <c r="C211">
+        <v>0.11</v>
+      </c>
+      <c r="D211">
+        <f ca="1">SUM(C$3:$D211)</f>
+        <v>95.280000000000086</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>4899</v>
+      </c>
+      <c r="B212">
+        <v>9</v>
+      </c>
+      <c r="C212">
+        <v>0.11</v>
+      </c>
+      <c r="D212">
+        <f ca="1">SUM(C$3:$D212)</f>
+        <v>95.390000000000086</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>4950</v>
+      </c>
+      <c r="B213">
+        <v>9</v>
+      </c>
+      <c r="C213">
+        <v>0.11</v>
+      </c>
+      <c r="D213">
+        <f ca="1">SUM(C$3:$D213)</f>
+        <v>95.500000000000085</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>5051</v>
+      </c>
+      <c r="B214">
+        <v>9</v>
+      </c>
+      <c r="C214">
+        <v>0.11</v>
+      </c>
+      <c r="D214">
+        <f ca="1">SUM(C$3:$D214)</f>
+        <v>95.610000000000085</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>5063</v>
+      </c>
+      <c r="B215">
+        <v>9</v>
+      </c>
+      <c r="C215">
+        <v>0.11</v>
+      </c>
+      <c r="D215">
+        <f ca="1">SUM(C$3:$D215)</f>
+        <v>95.720000000000084</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>5140</v>
+      </c>
+      <c r="B216">
+        <v>9</v>
+      </c>
+      <c r="C216">
+        <v>0.11</v>
+      </c>
+      <c r="D216">
+        <f ca="1">SUM(C$3:$D216)</f>
+        <v>95.830000000000084</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>5141</v>
+      </c>
+      <c r="B217">
+        <v>9</v>
+      </c>
+      <c r="C217">
+        <v>0.11</v>
+      </c>
+      <c r="D217">
+        <f ca="1">SUM(C$3:$D217)</f>
+        <v>95.940000000000083</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>5150</v>
+      </c>
+      <c r="B218">
+        <v>9</v>
+      </c>
+      <c r="C218">
+        <v>0.11</v>
+      </c>
+      <c r="D218">
+        <f ca="1">SUM(C$3:$D218)</f>
+        <v>96.050000000000082</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>5600</v>
+      </c>
+      <c r="B219">
+        <v>9</v>
+      </c>
+      <c r="C219">
+        <v>0.11</v>
+      </c>
+      <c r="D219">
+        <f ca="1">SUM(C$3:$D219)</f>
+        <v>96.160000000000082</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>5700</v>
+      </c>
+      <c r="B220">
+        <v>9</v>
+      </c>
+      <c r="C220">
+        <v>0.11</v>
+      </c>
+      <c r="D220">
+        <f ca="1">SUM(C$3:$D220)</f>
+        <v>96.270000000000081</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>5734</v>
+      </c>
+      <c r="B221">
+        <v>9</v>
+      </c>
+      <c r="C221">
+        <v>0.11</v>
+      </c>
+      <c r="D221">
+        <f ca="1">SUM(C$3:$D221)</f>
+        <v>96.380000000000081</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>5990</v>
+      </c>
+      <c r="B222">
+        <v>9</v>
+      </c>
+      <c r="C222">
+        <v>0.11</v>
+      </c>
+      <c r="D222">
+        <f ca="1">SUM(C$3:$D222)</f>
+        <v>96.49000000000008</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>6199</v>
+      </c>
+      <c r="B223">
+        <v>9</v>
+      </c>
+      <c r="C223">
+        <v>0.11</v>
+      </c>
+      <c r="D223">
+        <f ca="1">SUM(C$3:$D223)</f>
+        <v>96.60000000000008</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>6361</v>
+      </c>
+      <c r="B224">
+        <v>9</v>
+      </c>
+      <c r="C224">
+        <v>0.11</v>
+      </c>
+      <c r="D224">
+        <f ca="1">SUM(C$3:$D224)</f>
+        <v>96.710000000000079</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>6795</v>
+      </c>
+      <c r="B225">
+        <v>9</v>
+      </c>
+      <c r="C225">
+        <v>0.11</v>
+      </c>
+      <c r="D225">
+        <f ca="1">SUM(C$3:$D225)</f>
+        <v>96.820000000000078</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>7331</v>
+      </c>
+      <c r="B226">
+        <v>9</v>
+      </c>
+      <c r="C226">
+        <v>0.11</v>
+      </c>
+      <c r="D226">
+        <f ca="1">SUM(C$3:$D226)</f>
+        <v>96.930000000000078</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>7363</v>
+      </c>
+      <c r="B227">
+        <v>9</v>
+      </c>
+      <c r="C227">
+        <v>0.11</v>
+      </c>
+      <c r="D227">
+        <f ca="1">SUM(C$3:$D227)</f>
+        <v>97.040000000000077</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>7381</v>
+      </c>
+      <c r="B228">
+        <v>9</v>
+      </c>
+      <c r="C228">
+        <v>0.11</v>
+      </c>
+      <c r="D228">
+        <f ca="1">SUM(C$3:$D228)</f>
+        <v>97.150000000000077</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>7830</v>
+      </c>
+      <c r="B229">
+        <v>9</v>
+      </c>
+      <c r="C229">
+        <v>0.11</v>
+      </c>
+      <c r="D229">
+        <f ca="1">SUM(C$3:$D229)</f>
+        <v>97.260000000000076</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>1623</v>
+      </c>
+      <c r="B230">
+        <v>8</v>
+      </c>
+      <c r="C230">
+        <v>0.09</v>
+      </c>
+      <c r="D230">
+        <f ca="1">SUM(C$3:$D230)</f>
+        <v>97.35000000000008</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>2050</v>
+      </c>
+      <c r="B231">
+        <v>8</v>
+      </c>
+      <c r="C231">
+        <v>0.09</v>
+      </c>
+      <c r="D231">
+        <f ca="1">SUM(C$3:$D231)</f>
+        <v>97.440000000000083</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>3430</v>
+      </c>
+      <c r="B232">
+        <v>8</v>
+      </c>
+      <c r="C232">
+        <v>0.09</v>
+      </c>
+      <c r="D232">
+        <f ca="1">SUM(C$3:$D232)</f>
+        <v>97.530000000000086</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>3440</v>
+      </c>
+      <c r="B233">
+        <v>8</v>
+      </c>
+      <c r="C233">
+        <v>0.09</v>
+      </c>
+      <c r="D233">
+        <f ca="1">SUM(C$3:$D233)</f>
+        <v>97.62000000000009</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>3829</v>
+      </c>
+      <c r="B234">
+        <v>8</v>
+      </c>
+      <c r="C234">
+        <v>0.09</v>
+      </c>
+      <c r="D234">
+        <f ca="1">SUM(C$3:$D234)</f>
+        <v>97.710000000000093</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>4955</v>
+      </c>
+      <c r="B235">
+        <v>8</v>
+      </c>
+      <c r="C235">
+        <v>0.09</v>
+      </c>
+      <c r="D235">
+        <f ca="1">SUM(C$3:$D235)</f>
+        <v>97.800000000000097</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>5047</v>
+      </c>
+      <c r="B236">
+        <v>8</v>
+      </c>
+      <c r="C236">
+        <v>0.09</v>
+      </c>
+      <c r="D236">
+        <f ca="1">SUM(C$3:$D236)</f>
+        <v>97.8900000000001</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>7340</v>
+      </c>
+      <c r="B237">
+        <v>8</v>
+      </c>
+      <c r="C237">
+        <v>0.09</v>
+      </c>
+      <c r="D237">
+        <f ca="1">SUM(C$3:$D237)</f>
+        <v>97.980000000000103</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>8060</v>
+      </c>
+      <c r="B238">
+        <v>8</v>
+      </c>
+      <c r="C238">
+        <v>0.09</v>
+      </c>
+      <c r="D238">
+        <f ca="1">SUM(C$3:$D238)</f>
+        <v>98.070000000000107</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>8071</v>
+      </c>
+      <c r="B239">
+        <v>8</v>
+      </c>
+      <c r="C239">
+        <v>0.09</v>
+      </c>
+      <c r="D239">
+        <f ca="1">SUM(C$3:$D239)</f>
+        <v>98.16000000000011</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>2421</v>
+      </c>
+      <c r="B240">
+        <v>7</v>
+      </c>
+      <c r="C240">
+        <v>0.08</v>
+      </c>
+      <c r="D240">
+        <f ca="1">SUM(C$3:$D240)</f>
+        <v>98.240000000000109</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>2721</v>
+      </c>
+      <c r="B241">
+        <v>7</v>
+      </c>
+      <c r="C241">
+        <v>0.08</v>
+      </c>
+      <c r="D241">
+        <f ca="1">SUM(C$3:$D241)</f>
+        <v>98.320000000000107</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>2771</v>
+      </c>
+      <c r="B242">
+        <v>7</v>
+      </c>
+      <c r="C242">
+        <v>0.08</v>
+      </c>
+      <c r="D242">
+        <f ca="1">SUM(C$3:$D242)</f>
+        <v>98.400000000000105</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>2800</v>
+      </c>
+      <c r="B243">
+        <v>7</v>
+      </c>
+      <c r="C243">
+        <v>0.08</v>
+      </c>
+      <c r="D243">
+        <f ca="1">SUM(C$3:$D243)</f>
+        <v>98.480000000000103</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>3390</v>
+      </c>
+      <c r="B244">
+        <v>7</v>
+      </c>
+      <c r="C244">
+        <v>0.08</v>
+      </c>
+      <c r="D244">
+        <f ca="1">SUM(C$3:$D244)</f>
+        <v>98.560000000000102</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>3944</v>
+      </c>
+      <c r="B245">
+        <v>7</v>
+      </c>
+      <c r="C245">
+        <v>0.08</v>
+      </c>
+      <c r="D245">
+        <f ca="1">SUM(C$3:$D245)</f>
+        <v>98.6400000000001</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>5013</v>
+      </c>
+      <c r="B246">
+        <v>7</v>
+      </c>
+      <c r="C246">
+        <v>0.08</v>
+      </c>
+      <c r="D246">
+        <f ca="1">SUM(C$3:$D246)</f>
+        <v>98.720000000000098</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>6036</v>
+      </c>
+      <c r="B247">
+        <v>7</v>
+      </c>
+      <c r="C247">
+        <v>0.08</v>
+      </c>
+      <c r="D247">
+        <f ca="1">SUM(C$3:$D247)</f>
+        <v>98.800000000000097</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>3651</v>
+      </c>
+      <c r="B248">
+        <v>6</v>
+      </c>
+      <c r="C248">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D248">
+        <f ca="1">SUM(C$3:$D248)</f>
+        <v>98.87000000000009</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>5172</v>
+      </c>
+      <c r="B249">
+        <v>6</v>
+      </c>
+      <c r="C249">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D249">
+        <f ca="1">SUM(C$3:$D249)</f>
+        <v>98.940000000000083</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>8050</v>
+      </c>
+      <c r="B250">
+        <v>6</v>
+      </c>
+      <c r="C250">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D250">
+        <f ca="1">SUM(C$3:$D250)</f>
+        <v>99.010000000000076</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>2033</v>
+      </c>
+      <c r="B251">
+        <v>5</v>
+      </c>
+      <c r="C251">
+        <v>0.06</v>
+      </c>
+      <c r="D251">
+        <f ca="1">SUM(C$3:$D251)</f>
+        <v>99.070000000000078</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>2430</v>
+      </c>
+      <c r="B252">
+        <v>5</v>
+      </c>
+      <c r="C252">
+        <v>0.06</v>
+      </c>
+      <c r="D252">
+        <f ca="1">SUM(C$3:$D252)</f>
+        <v>99.130000000000081</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>2990</v>
+      </c>
+      <c r="B253">
+        <v>5</v>
+      </c>
+      <c r="C253">
+        <v>0.06</v>
+      </c>
+      <c r="D253">
+        <f ca="1">SUM(C$3:$D253)</f>
+        <v>99.190000000000083</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>3140</v>
+      </c>
+      <c r="B254">
+        <v>5</v>
+      </c>
+      <c r="C254">
+        <v>0.06</v>
+      </c>
+      <c r="D254">
+        <f ca="1">SUM(C$3:$D254)</f>
+        <v>99.250000000000085</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>3310</v>
+      </c>
+      <c r="B255">
+        <v>5</v>
+      </c>
+      <c r="C255">
+        <v>0.06</v>
+      </c>
+      <c r="D255">
+        <f ca="1">SUM(C$3:$D255)</f>
+        <v>99.310000000000088</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>3580</v>
+      </c>
+      <c r="B256">
+        <v>5</v>
+      </c>
+      <c r="C256">
+        <v>0.06</v>
+      </c>
+      <c r="D256">
+        <f ca="1">SUM(C$3:$D256)</f>
+        <v>99.37000000000009</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>5945</v>
+      </c>
+      <c r="B257">
+        <v>5</v>
+      </c>
+      <c r="C257">
+        <v>0.06</v>
+      </c>
+      <c r="D257">
+        <f ca="1">SUM(C$3:$D257)</f>
+        <v>99.430000000000092</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>7310</v>
+      </c>
+      <c r="B258">
+        <v>5</v>
+      </c>
+      <c r="C258">
+        <v>0.06</v>
+      </c>
+      <c r="D258">
+        <f ca="1">SUM(C$3:$D258)</f>
+        <v>99.490000000000094</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>2520</v>
+      </c>
+      <c r="B259">
+        <v>4</v>
+      </c>
+      <c r="C259">
+        <v>0.05</v>
+      </c>
+      <c r="D259">
+        <f ca="1">SUM(C$3:$D259)</f>
+        <v>99.540000000000092</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>2780</v>
+      </c>
+      <c r="B260">
+        <v>4</v>
+      </c>
+      <c r="C260">
+        <v>0.05</v>
+      </c>
+      <c r="D260">
+        <f ca="1">SUM(C$3:$D260)</f>
+        <v>99.590000000000089</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>2950</v>
+      </c>
+      <c r="B261">
+        <v>4</v>
+      </c>
+      <c r="C261">
+        <v>0.05</v>
+      </c>
+      <c r="D261">
+        <f ca="1">SUM(C$3:$D261)</f>
+        <v>99.640000000000086</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>3357</v>
+      </c>
+      <c r="B262">
+        <v>4</v>
+      </c>
+      <c r="C262">
+        <v>0.05</v>
+      </c>
+      <c r="D262">
+        <f ca="1">SUM(C$3:$D262)</f>
+        <v>99.690000000000083</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>3600</v>
+      </c>
+      <c r="B263">
+        <v>4</v>
+      </c>
+      <c r="C263">
+        <v>0.05</v>
+      </c>
+      <c r="D263">
+        <f ca="1">SUM(C$3:$D263)</f>
+        <v>99.74000000000008</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>4941</v>
+      </c>
+      <c r="B264">
+        <v>4</v>
+      </c>
+      <c r="C264">
+        <v>0.05</v>
+      </c>
+      <c r="D264">
+        <f ca="1">SUM(C$3:$D264)</f>
+        <v>99.790000000000077</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>2750</v>
+      </c>
+      <c r="B265">
+        <v>3</v>
+      </c>
+      <c r="C265">
+        <v>0.04</v>
+      </c>
+      <c r="D265">
+        <f ca="1">SUM(C$3:$D265)</f>
+        <v>99.830000000000084</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>3571</v>
+      </c>
+      <c r="B266">
+        <v>3</v>
+      </c>
+      <c r="C266">
+        <v>0.04</v>
+      </c>
+      <c r="D266">
+        <f ca="1">SUM(C$3:$D266)</f>
+        <v>99.87000000000009</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>7996</v>
+      </c>
+      <c r="B267">
+        <v>3</v>
+      </c>
+      <c r="C267">
+        <v>0.04</v>
+      </c>
+      <c r="D267">
+        <f ca="1">SUM(C$3:$D267)</f>
+        <v>99.910000000000096</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>2100</v>
+      </c>
+      <c r="B268">
+        <v>2</v>
+      </c>
+      <c r="C268">
+        <v>0.02</v>
+      </c>
+      <c r="D268">
+        <f ca="1">SUM(C$3:$D268)</f>
+        <v>99.930000000000092</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>3562</v>
+      </c>
+      <c r="B269">
+        <v>2</v>
+      </c>
+      <c r="C269">
+        <v>0.02</v>
+      </c>
+      <c r="D269">
+        <f ca="1">SUM(C$3:$D269)</f>
+        <v>99.950000000000088</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>3652</v>
+      </c>
+      <c r="B270">
+        <v>2</v>
+      </c>
+      <c r="C270">
+        <v>0.02</v>
+      </c>
+      <c r="D270">
+        <f ca="1">SUM(C$3:$D270)</f>
+        <v>99.970000000000084</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <v>4513</v>
+      </c>
+      <c r="B271">
+        <v>2</v>
+      </c>
+      <c r="C271">
+        <v>0.02</v>
+      </c>
+      <c r="D271">
+        <f ca="1">SUM(C$3:$D271)</f>
+        <v>99.99000000000008</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>6552</v>
+      </c>
+      <c r="B272">
+        <v>2</v>
+      </c>
+      <c r="C272">
+        <v>0.02</v>
+      </c>
+      <c r="D272">
+        <f ca="1">SUM(C$3:$D272)</f>
+        <v>100.01000000000008</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>2015</v>
+      </c>
+      <c r="B273">
+        <v>1</v>
+      </c>
+      <c r="C273">
+        <v>0.01</v>
+      </c>
+      <c r="D273">
+        <f ca="1">SUM(C$3:$D273)</f>
+        <v>100.02000000000008</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>3341</v>
+      </c>
+      <c r="B274">
+        <v>1</v>
+      </c>
+      <c r="C274">
+        <v>0.01</v>
+      </c>
+      <c r="D274">
+        <f ca="1">SUM(C$3:$D274)</f>
+        <v>100.03000000000009</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>6162</v>
+      </c>
+      <c r="B275">
+        <v>1</v>
+      </c>
+      <c r="C275">
+        <v>0.01</v>
+      </c>
+      <c r="D275">
+        <f ca="1">SUM(C$3:$D275)</f>
+        <v>100.04000000000009</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>6797</v>
+      </c>
+      <c r="B276">
+        <v>1</v>
+      </c>
+      <c r="C276">
+        <v>0.01</v>
+      </c>
+      <c r="D276">
+        <f ca="1">SUM(C$3:$D276)</f>
+        <v>100.0500000000001</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>7900</v>
+      </c>
+      <c r="B277">
+        <v>1</v>
+      </c>
+      <c r="C277">
+        <v>0.01</v>
+      </c>
+      <c r="D277">
+        <f ca="1">SUM(C$3:$D277)</f>
+        <v>100.0600000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100933D471B36D32045A644F96A039670B8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a0ea1f51b23783c55cd9af094bd05302">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c0e4948a-5198-4317-a521-447d65034b9e" xmlns:ns4="7944c567-076b-402f-96ab-e7aacbd2d542" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c4ff65db638d551b108ff03facd8731e" ns3:_="" ns4:_="">
     <xsd:import namespace="c0e4948a-5198-4317-a521-447d65034b9e"/>
@@ -4845,22 +9037,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A890B0FE-86CC-49B4-8067-A367AAA899E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98FD93DA-0E5E-4CE4-9E03-63A268F9B126}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72757EFF-1BA5-43B1-A312-9DD2FC80E9A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4877,21 +9071,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A890B0FE-86CC-49B4-8067-A367AAA899E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98FD93DA-0E5E-4CE4-9E03-63A268F9B126}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>